<commit_message>
Update the card importers with new address requirements
</commit_message>
<xml_diff>
--- a/templates/Tokenized Credit Cards.xlsx
+++ b/templates/Tokenized Credit Cards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -33,8 +33,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>Some payment processors create a customer profile when tokenizing cards. If your payment processor does this, add the profile identifier here.</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Some payment processors create a customer profile when tokenizing cards. If your payment processor does this, add the profile identifier here.</t>
         </r>
       </text>
     </comment>
@@ -45,8 +46,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>The tokenized string.</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The tokenized string.</t>
         </r>
       </text>
     </comment>
@@ -57,8 +59,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>Some method of identifying the card. Typically the last 4 digits of the card.</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Some method of identifying the card. Typically the last 4 digits of the card.</t>
         </r>
       </text>
     </comment>
@@ -69,8 +72,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>4 digit expiration year (e.g. 2020)</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">4 digit expiration year (e.g. 2020)</t>
         </r>
       </text>
     </comment>
@@ -81,8 +85,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>Two digit expiration month (e.g. 09)</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Two digit expiration month (e.g. 09)</t>
         </r>
       </text>
     </comment>
@@ -93,8 +98,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>1 if this card should be set for autopay. 0 if not.</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">1 if this card should be set for autopay. 0 if not.</t>
         </r>
       </text>
     </comment>
@@ -105,8 +111,35 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>Card type, one of "visaelectron", "maestro", "forbrugsforeningen", "dankort", "visa", "mastercard", "amex", "dinersclub", "discover", "unionpay", "jcb"</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Card type, one of "visaelectron", "maestro", "forbrugsforeningen", "dankort", "visa", "mastercard", "amex", "dinersclub", "discover", "unionpay", "jcb"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Must be a supported subdivision from the Sonar list. This is the two character code for the US and Canada (e.g. WI, NY, AB)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Must be a two character code (US, CA, GB)</t>
         </r>
       </text>
     </comment>
@@ -115,30 +148,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Account ID</t>
-  </si>
-  <si>
-    <t>Payment Processor Customer Profile ID</t>
-  </si>
-  <si>
-    <t>Token</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>Expiration Year</t>
-  </si>
-  <si>
-    <t>Expiration Month</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Card Type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Account ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment Processor Customer Profile ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expiration Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expiration Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Card Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name on card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
   </si>
 </sst>
 </file>
@@ -146,13 +197,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -172,13 +224,14 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -330,20 +383,20 @@
       <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="50040" y="19080"/>
-          <a:ext cx="8067960" cy="6014520"/>
+          <a:ext cx="7953120" cy="6014160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -355,28 +408,80 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>This sheet allows importing of existing, tokenized credit cards. Be cautious when using this – you must ensure the tokens are valid for the payment processor you are currently using, as Sonar has no way of validating this.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Grey headers are required, blue are potentially optional, please read the comments on each column.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -393,12 +498,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+      <selection pane="topLeft" activeCell="M18" activeCellId="1" sqref="I1:N1 M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -417,21 +522,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,11 +568,29 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>